<commit_message>
Documentation of V0.7.0 beta finished
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="28515" windowHeight="14895"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="25440" windowHeight="14895"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -197,6 +197,27 @@
   </si>
   <si>
     <t>This idea was broght forward by Tom Glenn on the Cloudy Nights forum.</t>
+  </si>
+  <si>
+    <t>Bug if the user wants to go back to a previous step after a job is aborted</t>
+  </si>
+  <si>
+    <t>If a job is aborted because of a runtime error, execution continues with the next job, or the program is set to idle mode (if there are no more jobs). If then the user presses "go back to" he is presented with the full set of job steps to choose from, even if they have not been executed for the aborted job. If he then chooses a step which was not executed, the program crashes without further notice.</t>
+  </si>
+  <si>
+    <t>The job control in the main GUI thread must be corrected.</t>
+  </si>
+  <si>
+    <t>Bug fix</t>
+  </si>
+  <si>
+    <t>Add the option to manually exclude frames from the input stack</t>
+  </si>
+  <si>
+    <t>This should be added to the phase where the stack size is set. When the user scrolls through the video (using the slider or the number boxes), an additional checkbox can be set / unset to include / exclude a given frame from the input stack.</t>
+  </si>
+  <si>
+    <t>The implementation should be done in the module "frames" via an index translation table. This way (by going back to this step) frames can be restored by simply resetting the translation table.</t>
   </si>
 </sst>
 </file>
@@ -282,13 +303,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -337,13 +358,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -667,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,22 +764,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
@@ -767,15 +788,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
@@ -791,15 +812,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
@@ -815,17 +836,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>24</v>
@@ -837,19 +860,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>24</v>
@@ -858,20 +879,22 @@
         <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>24</v>
@@ -880,22 +903,20 @@
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>24</v>
@@ -904,18 +925,18 @@
         <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
@@ -931,46 +952,46 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>35</v>
@@ -979,17 +1000,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="405" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1003,17 +1024,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1027,25 +1048,53 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+    <row r="16" spans="1:8" ht="405" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -1106,6 +1155,26 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Bug fixed if going back after aborted job, context menu restricted to video files, roadmap updated
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -214,10 +214,25 @@
     <t>Add the option to manually exclude frames from the input stack</t>
   </si>
   <si>
-    <t>This should be added to the phase where the stack size is set. When the user scrolls through the video (using the slider or the number boxes), an additional checkbox can be set / unset to include / exclude a given frame from the input stack.</t>
-  </si>
-  <si>
     <t>The implementation should be done in the module "frames" via an index translation table. This way (by going back to this step) frames can be restored by simply resetting the translation table.</t>
+  </si>
+  <si>
+    <t>&gt; 0.7.0?</t>
+  </si>
+  <si>
+    <t>This should be added as an additional phase (only in interactive mode) before the stack size is set. The GUI looks very similar to the stack size selection window. Instead of the Matplotlib window with frame qualities, a list of all frames is presented. The user can select / deselect frames in this list.</t>
+  </si>
+  <si>
+    <t>0.8.0</t>
+  </si>
+  <si>
+    <t>Add the option to use the "delete" key in the job editor instead of pressing the "remove selected job(s)" button explicitly</t>
+  </si>
+  <si>
+    <t>So far, when the user selects some job entries and presses the "del" key, nothing happens. This should be added as an alternative to using the "remove selected job(s)" key underneath the job list window.</t>
+  </si>
+  <si>
+    <t>Probably many users will expect this functionality to work.</t>
   </si>
 </sst>
 </file>
@@ -303,13 +318,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -358,13 +373,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -688,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,63 +779,63 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
@@ -836,15 +851,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
@@ -860,17 +875,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>24</v>
@@ -879,22 +896,20 @@
         <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>24</v>
@@ -908,15 +923,17 @@
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>24</v>
@@ -928,19 +945,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>24</v>
@@ -949,18 +964,18 @@
         <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
@@ -976,65 +991,65 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1042,23 +1057,23 @@
         <v>34</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="405" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1072,17 +1087,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="405" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
@@ -1090,21 +1105,35 @@
         <v>34</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+    <row r="18" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1175,6 +1204,16 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
png saving added, debayer code BGR added
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>0.7.0</t>
-  </si>
-  <si>
-    <t>Michal</t>
   </si>
   <si>
     <t>User Guide update</t>
@@ -76,23 +73,6 @@
     <t>I will start a discussion on Cloudy Nights to find someone to help with the details.</t>
   </si>
   <si>
-    <t>Documentation of I/O file formats</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Michal: please enter details under "Description". In particular: which document are you talking about?
-In the user guide document, only the lists of possible choices should be included. No internal details.</t>
-  </si>
-  <si>
-    <t>Documentation of Debayering</t>
-  </si>
-  <si>
-    <t>Michal: please enter details under "Description". In particular: which document are you talking about?
-The user guide document already contains a description of how to select the debayering scheme.</t>
-  </si>
-  <si>
     <t>Importance</t>
   </si>
   <si>
@@ -138,10 +118,6 @@
     <t>Debayering during dark / flat file import</t>
   </si>
   <si>
-    <t>We must clarify how dark and flat frames which are read from the file system are treated with respect to debayering. Do we assume that those files are produced in a previous PSS run, so we know their internal formatting? Or do we assume that they are any FITS / TIFF files for which the user should be able to specify a different debayering pattern?
-If so, do we need to add the possibility to select the pattern through an additional menu entry? Or do we assume that the "standard" debayering option selected in the configuration dialog should be applied here? If we want to support non-standard debayering here at all, I would opt for this latter option, because it is the same way debayering is selected when a dark / flat frame is to be produced in PSS from video input.</t>
-  </si>
-  <si>
     <t>Applying a non-standard debayering pattern can be as useful for dark / flat frames as for the videos / image folders to be stacked. It is unclear how PSS treats the case when dark / flat frames are read from the file system.
 We need at least a clarification here, possibly also an addition in the SW.</t>
   </si>
@@ -233,6 +209,21 @@
   </si>
   <si>
     <t>Probably many users will expect this functionality to work.</t>
+  </si>
+  <si>
+    <t>Not clear if necessary at all</t>
+  </si>
+  <si>
+    <t>Add a brightness control to postproc editor</t>
+  </si>
+  <si>
+    <t>The control should only change the brightness of the display. It should not affect the content of the output file.</t>
+  </si>
+  <si>
+    <t>John Duchek asked for this feature. If the videos are quite dark, it is hard to judge the effect of postprocessing in the editor.</t>
+  </si>
+  <si>
+    <t>We must clarify how dark and flat frames which are read from the file system are treated with respect to debayering. We assume that the files have been produced in a previous PSS run, so non-standard debayering is not necessary in this case.</t>
   </si>
 </sst>
 </file>
@@ -318,13 +309,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -373,13 +364,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -703,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,103 +737,103 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -851,46 +842,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="315" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>10</v>
@@ -901,10 +868,10 @@
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -912,37 +879,37 @@
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -958,181 +925,181 @@
         <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="405" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="405" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1204,16 +1171,6 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Improved frame normalization, GUI adapted
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Implementation of Debayering in VideoReader</t>
   </si>
   <si>
-    <t>The selection of debayering patterns is alredy implemented in the GUI. It is passed to the VideoReader initialization via the instance variable "self.debayer_pattern". All supported patterns should be recognized and implemented in the read_frame method.</t>
-  </si>
-  <si>
     <t>Is there anything still missing?</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
   <si>
     <t>The selection of debayering patterns is alredy implemented in the GUI. It is passed to the ImageReader initialization via the instance variable "self.debayer_pattern". All supported patterns should be recognized and implemented in the read_frame method.
 So far, the variable "self.debayer_pattern" is not used.</t>
-  </si>
-  <si>
-    <t>Michal: Do you see any technical problems with this task?</t>
   </si>
   <si>
     <t>Add the frame stabilization mode "None"</t>
@@ -129,10 +123,6 @@
     <t>Debayering during dark / flat file import</t>
   </si>
   <si>
-    <t>We must clarify how dark and flat frames which are read from the file system are treated with respect to debayering. Do we assume that those files are produced in a previous PSS run, so we know their internal formatting? Or do we assume that they are any FITS / TIFF files for which the user should be able to specify a different debayering pattern?
-If so, do we need to add the possibility to select the pattern through an additional menu entry? Or do we assume that the "standard" debayering option selected in the configuration dialog should be applied here? If we want to support non-standard debayering here at all, I would opt for this latter option, because it is the same way debayering is selected when a dark / flat frame is to be produced in PSS from video input.</t>
-  </si>
-  <si>
     <t>Applying a non-standard debayering pattern can be as useful for dark / flat frames as for the videos / image folders to be stacked. It is unclear how PSS treats the case when dark / flat frames are read from the file system.
 We need at least a clarification here, possibly also an addition in the SW.</t>
   </si>
@@ -236,6 +226,22 @@
   </si>
   <si>
     <t>Rolf (plus John Duchek from the Cloudy Nights forum)</t>
+  </si>
+  <si>
+    <t>We assume that still image files are debayered already.</t>
+  </si>
+  <si>
+    <t>The selection of debayering patterns is alredy implemented in the GUI. It is passed to the VideoReader initialization via the instance variable "self.debayer_pattern". All supported patterns should be recognized and implemented in the read_frame method. Automatic detection of bayer matrices is implemented as well as the automatic detection of RGB channel ordering.</t>
+  </si>
+  <si>
+    <t>Frame brightness normalization</t>
+  </si>
+  <si>
+    <t>So far, only the related images (grayscale, Gauss, etc.) are normalized, such that the evaluation is not misled by brightness variations.
+Normalization should also be implemented for frame stacking. This will reduce blending artifacts.</t>
+  </si>
+  <si>
+    <t>The derived frame types should not be changed at all. Only the brightnesses are stored as a single value per frame. This will reduce compute times and limit clipping defects. Also, normalization should be made optional by adding GUI parameters.</t>
   </si>
 </sst>
 </file>
@@ -321,13 +327,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -376,13 +382,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -706,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,18 +757,18 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -774,87 +780,87 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -866,18 +872,18 @@
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
@@ -889,17 +895,19 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
@@ -910,21 +918,19 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>21</v>
@@ -933,19 +939,21 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>21</v>
@@ -954,19 +962,17 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
@@ -977,178 +983,192 @@
         <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="285" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="F19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="405" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1212,6 +1232,15 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Viewer image brightness normalized
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Targeted for Version</t>
-  </si>
-  <si>
-    <t>Discussion Rolf</t>
   </si>
   <si>
     <t>Author Responsible</t>
@@ -177,18 +174,6 @@
     <t>This idea was broght forward by Tom Glenn on the Cloudy Nights forum.</t>
   </si>
   <si>
-    <t>Bug if the user wants to go back to a previous step after a job is aborted</t>
-  </si>
-  <si>
-    <t>If a job is aborted because of a runtime error, execution continues with the next job, or the program is set to idle mode (if there are no more jobs). If then the user presses "go back to" he is presented with the full set of job steps to choose from, even if they have not been executed for the aborted job. If he then chooses a step which was not executed, the program crashes without further notice.</t>
-  </si>
-  <si>
-    <t>The job control in the main GUI thread must be corrected.</t>
-  </si>
-  <si>
-    <t>Bug fix</t>
-  </si>
-  <si>
     <t>Add the option to manually exclude frames from the input stack</t>
   </si>
   <si>
@@ -242,6 +227,37 @@
   </si>
   <si>
     <t>The derived frame types should not be changed at all. Only the brightnesses are stored as a single value per frame. This will reduce compute times and limit clipping defects. Also, normalization should be made optional by adding GUI parameters.</t>
+  </si>
+  <si>
+    <t>Automatically adjust the image brightness in the frame viewers during the workflow  (without changing the image content), so that the pixel values cover the entire dynamic range.</t>
+  </si>
+  <si>
+    <t>Automatic image brightness adjustment in frame viewers</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Simply spread the brightness distribution of pixels such that the minimum is zero and the maximum is 255. The method should work both for grayscale and color images.</t>
+  </si>
+  <si>
+    <t>Add multi-size AP option</t>
+  </si>
+  <si>
+    <t>Especially in moon videos usually there are large areas with little structure (maria). With standard AP sizes this leads to large holes in the AP grid. Adding larger AP patches there manually is tedious. It would be nice if they could be added automatically.</t>
+  </si>
+  <si>
+    <t>This can be implemented either as multiple rounds of AP creation (with different sizes) or by adapting the AP creation process individually: If an AP creation fails because the structure or brightness condition is violated, PSS tries again using a larger AP size. This is continued (up to some threshold) until the AP conditions are fulfilled.</t>
+  </si>
+  <si>
+    <t>Add "drizzle" support</t>
+  </si>
+  <si>
+    <t>Increase the pixel resolution by factors of 1.5 or 3 in both coordinate directions.</t>
+  </si>
+  <si>
+    <t>Some planetary observers use this feature prior to postprocessing even if the input videos are oversampled already.
+It is not clear yet at which phase in the workflow the image size is to be enlarged (before stacking, or just before postprocessing).</t>
   </si>
 </sst>
 </file>
@@ -327,13 +343,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -382,13 +398,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -712,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,448 +761,476 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="G12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="G16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="G20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="285" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="405" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1241,6 +1285,24 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
dynamic range correction for darks/flats
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="150" windowWidth="25440" windowHeight="14895"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Version 0.7.0" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="77">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -258,6 +258,16 @@
   <si>
     <t>Some planetary observers use this feature prior to postprocessing even if the input videos are oversampled already.
 It is not clear yet at which phase in the workflow the image size is to be enlarged (before stacking, or just before postprocessing).</t>
+  </si>
+  <si>
+    <t>Shift video frame pixel values to fully use 16bit dynamic range</t>
+  </si>
+  <si>
+    <t>The metadata of SER videos often do not reflect the actual video data. In particular, the value "PixelDepthPerPlane" is often wrong for 16bit input, i.e. it is set to 16, but the video data only use the lower 8, 10 or 12 bit. If not corrected, the stacked output would alsmost be black.
+This kind of error needs to be detected automatically, and video data must be left-shifted by the appropriate amount of bits to fully use the dynamic range of 16 bits.</t>
+  </si>
+  <si>
+    <t>Add a method "correct_dynamic_range" to the SER parser. For 16bit input it determines the maximal pixel values in three frames (first, middle of video, last) during file opening, and the number of unused (high) bits. Later, when frames are read, the content is left-shifted by this number of bits.</t>
   </si>
 </sst>
 </file>
@@ -343,13 +353,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -398,13 +408,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -728,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,21 +809,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>8</v>
@@ -822,21 +832,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>8</v>
@@ -845,15 +855,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -868,21 +878,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
@@ -891,15 +901,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -914,16 +924,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
@@ -934,21 +942,21 @@
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>20</v>
@@ -960,12 +968,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -978,24 +986,24 @@
         <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>8</v>
@@ -1004,19 +1012,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>8</v>
@@ -1025,47 +1035,47 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>33</v>
@@ -1073,13 +1083,13 @@
     </row>
     <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -1094,15 +1104,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -1117,44 +1127,44 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>48</v>
@@ -1163,15 +1173,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
@@ -1180,21 +1190,21 @@
         <v>28</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -1203,21 +1213,21 @@
         <v>28</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="405" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -1226,20 +1236,34 @@
         <v>28</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+    <row r="23" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1303,6 +1327,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated setup_*.py files and PyPI instructions after uploading version 0.8.0b13
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="89">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -264,9 +264,6 @@
     <t>In this processing mode, "automatic" processing is switched on. In other words: There is no user interaction via a GUI possible.</t>
   </si>
   <si>
-    <t>&gt; 0.8.0</t>
-  </si>
-  <si>
     <t>Improve buffer handling</t>
   </si>
   <si>
@@ -295,6 +292,15 @@
   </si>
   <si>
     <t>Currently the frame exclusion takes place before the frame ranks are computed. So, the only available ordering is chronological. The dialog must be delayed until ranks are available. The best solution seems to be to include the dialog with the setting of the stacking rate.</t>
+  </si>
+  <si>
+    <t>0.9.0</t>
+  </si>
+  <si>
+    <t>The solution in V0.8.0 does not work in interactive mode. If the data objects are referenced both from the workflow and GUI threads they are not deleted at the beginning of the next job.</t>
+  </si>
+  <si>
+    <t>&gt; 0.9.0</t>
   </si>
 </sst>
 </file>
@@ -380,13 +386,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -435,13 +441,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -765,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,19 +1093,19 @@
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>43</v>
@@ -1154,15 +1160,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
@@ -1171,53 +1177,53 @@
         <v>15</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>27</v>
@@ -1225,13 +1231,13 @@
     </row>
     <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -1240,21 +1246,21 @@
         <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -1263,21 +1269,21 @@
         <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
@@ -1286,21 +1292,21 @@
         <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1309,21 +1315,21 @@
         <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
@@ -1332,21 +1338,21 @@
         <v>23</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="405" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1355,20 +1361,34 @@
         <v>23</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+    <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1432,6 +1452,15 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
User Guide document ready for Release 0.8.0
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -301,6 +301,33 @@
   </si>
   <si>
     <t>&gt; 0.9.0</t>
+  </si>
+  <si>
+    <t>Improve RAM de-allocation</t>
+  </si>
+  <si>
+    <t>Automatic buffering mode</t>
+  </si>
+  <si>
+    <t>Add the option "auto" to the buffering level selection. In this case PSS selects the highest possible buffering level automatically at the beginning of each job.</t>
+  </si>
+  <si>
+    <t>"auto" should become the default option. The manual selection of a fixed level should still be possible.</t>
+  </si>
+  <si>
+    <t>Improve "planet" stabilization mode in the presence of a bright background</t>
+  </si>
+  <si>
+    <t>If the background is bright the "center of mass" computation for frame stabilization ("Planet" mode) can be unreliable.</t>
+  </si>
+  <si>
+    <t>The following strategy could help:
+- Deterimine the background brightness.
+- set a threshold a little higher .
+- Ignore all pixels up to this threshold in the "CoG" computation.</t>
+  </si>
+  <si>
+    <t>&gt; 0.8.0</t>
   </si>
 </sst>
 </file>
@@ -386,13 +413,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -441,13 +468,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -771,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1235,7 @@
     </row>
     <row r="20" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>77</v>
@@ -1229,38 +1256,38 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -1269,21 +1296,21 @@
         <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
@@ -1298,15 +1325,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1321,15 +1348,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
@@ -1344,15 +1371,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1367,15 +1394,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
@@ -1390,23 +1417,51 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+    <row r="28" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1461,6 +1516,24 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Documentation updated, upgraded to version 0.8.14
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="105">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -336,13 +336,23 @@
     <t>MKL is used in Numpy and OpenCV. Its performance is critical for PSS. So far, it seems that several cores are reserved in MKL, but at any given time only one is active.</t>
   </si>
   <si>
-    <t>Change postprocessing to make it identical to Registax 6</t>
-  </si>
-  <si>
-    <t>Having the same user interface and processing algorithms would help users who so far used PSS for stacking only and did the postprocessing in Registax 6.</t>
-  </si>
-  <si>
-    <t>The sharpening filters used in Registax 6 and PSS are the same already now. Only their application to the different wavelet levels is different. Changing the PSS behaviour to make it identical to Registax is easy from the algorithmic point of view. The largest fraction of the work is changing the GUI.</t>
+    <t>George / Rolf</t>
+  </si>
+  <si>
+    <t>Improve postprocessing</t>
+  </si>
+  <si>
+    <t>The goal is make postprocessing better than Registax 6, both in terms of functionality and resulting image quality.</t>
+  </si>
+  <si>
+    <t>Alex / Rolf</t>
+  </si>
+  <si>
+    <t>The sharpening filters used in Registax 6 and PSS are the same already now. Only their application to the different wavelet levels is different. Changing the PSS behaviour to make it identical to Registax is easy from the algorithmic point of view. The largest fraction of the work is changing the GUI.
+Additional to the Registax functionality new filters should be made available, as, for example, bilateral filtering.</t>
+  </si>
+  <si>
+    <t>George ?</t>
   </si>
 </sst>
 </file>
@@ -815,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1269,7 @@
         <v>87</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>79</v>
@@ -1268,7 +1278,7 @@
         <v>86</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1317,24 +1327,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>27</v>
@@ -1351,13 +1361,13 @@
         <v>98</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>27</v>
@@ -1373,9 +1383,7 @@
       <c r="C25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1396,9 +1404,7 @@
       <c r="C26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1419,9 +1425,7 @@
       <c r="C27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>23</v>
       </c>
@@ -1442,9 +1446,7 @@
       <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
         <v>23</v>
       </c>
@@ -1465,9 +1467,7 @@
       <c r="C29" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
         <v>23</v>
       </c>
@@ -1488,9 +1488,7 @@
       <c r="C30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1511,9 +1509,7 @@
       <c r="C31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
algorithm summary and roadmap updated
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="114">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t>George</t>
+  </si>
+  <si>
+    <t>Improve zoom function in image viewer</t>
+  </si>
+  <si>
+    <t>Users criticize that there is no info shown about the current zoom status, and that there is no easy way to set the zoom status to 100%.</t>
+  </si>
+  <si>
+    <t>The zoom status should be included in one of the viewer corners (upper right?), e.g. "125%". Additionally, pressing "1" or double-clicking on the viewer image should reset to 100%.</t>
   </si>
 </sst>
 </file>
@@ -487,13 +496,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -542,13 +551,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -872,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,22 +1477,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E27" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>27</v>
@@ -1491,13 +1502,13 @@
     </row>
     <row r="28" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
@@ -1510,15 +1521,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
@@ -1531,15 +1542,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
@@ -1552,15 +1563,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
@@ -1573,15 +1584,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
@@ -1594,15 +1605,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="405" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
@@ -1615,14 +1626,26 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+    <row r="34" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -1686,6 +1709,15 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Error message moved from stdout to stderr, object parents changed to None.
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SW-Development\Python\PlanetarySystemStacker\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D0B79-B0D9-4AD4-A428-4BA2CA0DDEFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="25440" windowHeight="14895"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="25440" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 0.7.0" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="116">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -401,11 +407,20 @@
   <si>
     <t>The zoom status should be included in one of the viewer corners (upper right?), e.g. "125%". Additionally, pressing "1" or double-clicking on the viewer image should reset to 100%.</t>
   </si>
+  <si>
+    <t>Implement parameter --stack_number</t>
+  </si>
+  <si>
+    <t>The parameter is accepted in pss_console.py, but it has no effect.</t>
+  </si>
+  <si>
+    <t>The problem is that PSS internally only works with "stack percent". This makes it hard to have an exact number of frames stacked. This has to be changed in the entire workflow.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,6 +498,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -493,18 +511,24 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Billede1"/>
+        <xdr:cNvPr id="3" name="Billede1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -548,18 +572,24 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Billede2"/>
+        <xdr:cNvPr id="5" name="Billede2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -592,9 +622,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -632,9 +662,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -667,9 +697,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,9 +749,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -877,10 +941,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1497,22 +1561,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E28" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>27</v>
@@ -1520,13 +1586,13 @@
     </row>
     <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
@@ -1539,15 +1605,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
@@ -1560,15 +1626,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
@@ -1581,15 +1647,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
@@ -1602,15 +1668,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
@@ -1623,15 +1689,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="405" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
@@ -1644,14 +1710,26 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+    <row r="35" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -1715,6 +1793,15 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1727,7 +1814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1739,7 +1826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
stack limit alternatively based on number and percentage of frames
</commit_message>
<xml_diff>
--- a/Documentation/Development_Roadmap.xlsx
+++ b/Documentation/Development_Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SW-Development\Python\PlanetarySystemStacker\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D0B79-B0D9-4AD4-A428-4BA2CA0DDEFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81B6A06-1FC7-469B-903C-1AEC254D11F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="25440" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="119">
   <si>
     <t>PlanetarySystemStacker: Development Roadmap</t>
   </si>
@@ -408,13 +408,23 @@
     <t>The zoom status should be included in one of the viewer corners (upper right?), e.g. "125%". Additionally, pressing "1" or double-clicking on the viewer image should reset to 100%.</t>
   </si>
   <si>
-    <t>Implement parameter --stack_number</t>
-  </si>
-  <si>
     <t>The parameter is accepted in pss_console.py, but it has no effect.</t>
   </si>
   <si>
-    <t>The problem is that PSS internally only works with "stack percent". This makes it hard to have an exact number of frames stacked. This has to be changed in the entire workflow.</t>
+    <t>Allow the stack size specification alternatively by number or percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So far the stack size is always computed from the percentage. Users want to be able to specify exact frame numbers.
+</t>
+  </si>
+  <si>
+    <t>Both the percentage and frame number must be configuration parameters with "equal rights". The one which is selected specifically gets a positive value, the other one -1. This way it can always be decided which of the two was specified by the user, and which one was derived from it (e.g. in the frame viewer where the stack size is entered.</t>
+  </si>
+  <si>
+    <t>The previous task must be done before thsi one.</t>
+  </si>
+  <si>
+    <t>Implement parameter --stack_number in the command line version of PSS</t>
   </si>
 </sst>
 </file>
@@ -511,13 +521,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1609725</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4953001</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>3175083</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -572,13 +582,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>1343024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4924425</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>4761229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -942,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1516,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>86</v>
@@ -1561,15 +1571,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
@@ -1581,39 +1591,41 @@
         <v>86</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="2"/>
+        <v>117</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
@@ -1626,15 +1638,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
@@ -1647,15 +1659,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
@@ -1668,15 +1680,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="285" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
@@ -1689,15 +1701,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
@@ -1710,15 +1722,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="405" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
@@ -1731,14 +1743,26 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+    <row r="36" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -1802,6 +1826,15 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>